<commit_message>
chore: update database.xlsx (add new driver)
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecommerce\Desktop\Pessoal Ricardo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\Downloads\f1-manager-light-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF600C18-46F6-4995-AE86-A5CCEDE4E9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4622997-A5F7-4431-807E-F08365E160A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="1050" windowWidth="21840" windowHeight="13740" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="driver_attribute_weights" sheetId="25" r:id="rId1"/>
@@ -53,15 +53,12 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3195" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3201" uniqueCount="761">
   <si>
     <t>key</t>
   </si>
@@ -2335,6 +2332,15 @@
   </si>
   <si>
     <t>layout</t>
+  </si>
+  <si>
+    <t>d_0029</t>
+  </si>
+  <si>
+    <t>Niki Lauda</t>
+  </si>
+  <si>
+    <t>AT</t>
   </si>
 </sst>
 </file>
@@ -2469,7 +2475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2490,16 +2496,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2884,70 +2887,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>729</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>444</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="11" t="s">
         <v>459</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="11" t="s">
         <v>461</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="11" t="s">
         <v>462</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="11" t="s">
         <v>463</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="11" t="s">
         <v>464</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V1" s="11" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5265,7 +5268,7 @@
       <c r="D1" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>394</v>
       </c>
     </row>
@@ -5573,10 +5576,10 @@
       <c r="G1" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>437</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>438</v>
       </c>
     </row>
@@ -6448,7 +6451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -6499,7 +6502,7 @@
       <c r="J1" s="7" t="s">
         <v>620</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>757</v>
       </c>
     </row>
@@ -6531,7 +6534,7 @@
       <c r="J2" s="5">
         <v>24</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="20" t="s">
         <v>756</v>
       </c>
     </row>
@@ -7345,25 +7348,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>40</v>
       </c>
     </row>
@@ -9523,16 +9526,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>718</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>720</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>721</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>719</v>
       </c>
     </row>
@@ -9616,53 +9619,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>412</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>413</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>414</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="19">
+      <c r="A2" s="18">
         <v>1980</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>416</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>417</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>418</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
+      <c r="A3" s="18">
         <v>1995</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>420</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>421</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>422</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>423</v>
       </c>
     </row>
@@ -9690,53 +9693,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>424</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>425</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>426</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="19">
+      <c r="A2" s="18">
         <v>1980</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>428</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>429</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>430</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
+      <c r="A3" s="18">
         <v>2000</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>432</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>433</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>434</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>435</v>
       </c>
     </row>
@@ -10058,26 +10061,26 @@
     <col min="11" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>479</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>539</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>534</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>535</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>475</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>704</v>
       </c>
     </row>
@@ -10263,10 +10266,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="A30" sqref="A30:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -10305,34 +10308,34 @@
       <c r="E1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>474</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>510</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>508</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>472</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>485</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>473</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>512</v>
       </c>
-      <c r="O1" s="10">
+      <c r="O1" s="9">
         <v>1980</v>
       </c>
     </row>
@@ -10406,14 +10409,14 @@
       <c r="H3" s="5">
         <v>1982</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="10">
         <v>37079</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>712</v>
       </c>
       <c r="N3" s="5" t="str">
-        <f t="shared" ref="N3:N29" si="0">IF($O$1 &lt; F3,
+        <f>IF($O$1 &lt; F3,
    "hidden",
    IF(AND(I3&lt;&gt;"", YEAR(I3) &lt;= $O$1),
       "deceased",
@@ -10454,14 +10457,26 @@
       <c r="H4" s="5">
         <v>1982</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="10">
         <v>30079</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>713</v>
       </c>
       <c r="N4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F4,
+   "hidden",
+   IF(AND(I4&lt;&gt;"", YEAR(I4) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G4,
+         "junior_only",
+         IF(OR(H4="", $O$1 &lt;= H4),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10494,7 +10509,19 @@
         <v>714</v>
       </c>
       <c r="N5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F5,
+   "hidden",
+   IF(AND(I5&lt;&gt;"", YEAR(I5) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G5,
+         "junior_only",
+         IF(OR(H5="", $O$1 &lt;= H5),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10524,7 +10551,19 @@
         <v>1991</v>
       </c>
       <c r="N6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F6,
+   "hidden",
+   IF(AND(I6&lt;&gt;"", YEAR(I6) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G6,
+         "junior_only",
+         IF(OR(H6="", $O$1 &lt;= H6),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10554,7 +10593,19 @@
         <v>1986</v>
       </c>
       <c r="N7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F7,
+   "hidden",
+   IF(AND(I7&lt;&gt;"", YEAR(I7) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G7,
+         "junior_only",
+         IF(OR(H7="", $O$1 &lt;= H7),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10583,11 +10634,23 @@
       <c r="H8" s="5">
         <v>1982</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <v>32012</v>
       </c>
       <c r="N8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F8,
+   "hidden",
+   IF(AND(I8&lt;&gt;"", YEAR(I8) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G8,
+         "junior_only",
+         IF(OR(H8="", $O$1 &lt;= H8),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10617,7 +10680,19 @@
         <v>1989</v>
       </c>
       <c r="N9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F9,
+   "hidden",
+   IF(AND(I9&lt;&gt;"", YEAR(I9) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G9,
+         "junior_only",
+         IF(OR(H9="", $O$1 &lt;= H9),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10646,11 +10721,23 @@
       <c r="H10" s="5">
         <v>1986</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <v>31547</v>
       </c>
       <c r="N10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F10,
+   "hidden",
+   IF(AND(I10&lt;&gt;"", YEAR(I10) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G10,
+         "junior_only",
+         IF(OR(H10="", $O$1 &lt;= H10),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10679,11 +10766,23 @@
       <c r="H11" s="5">
         <v>1981</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>44959</v>
       </c>
       <c r="N11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F11,
+   "hidden",
+   IF(AND(I11&lt;&gt;"", YEAR(I11) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G11,
+         "junior_only",
+         IF(OR(H11="", $O$1 &lt;= H11),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10713,7 +10812,19 @@
         <v>1993</v>
       </c>
       <c r="N12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F12,
+   "hidden",
+   IF(AND(I12&lt;&gt;"", YEAR(I12) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G12,
+         "junior_only",
+         IF(OR(H12="", $O$1 &lt;= H12),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10743,7 +10854,19 @@
         <v>1986</v>
       </c>
       <c r="N13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F13,
+   "hidden",
+   IF(AND(I13&lt;&gt;"", YEAR(I13) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G13,
+         "junior_only",
+         IF(OR(H13="", $O$1 &lt;= H13),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10773,7 +10896,19 @@
         <v>1985</v>
       </c>
       <c r="N14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F14,
+   "hidden",
+   IF(AND(I14&lt;&gt;"", YEAR(I14) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G14,
+         "junior_only",
+         IF(OR(H14="", $O$1 &lt;= H14),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10803,7 +10938,19 @@
         <v>1982</v>
       </c>
       <c r="N15" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F15,
+   "hidden",
+   IF(AND(I15&lt;&gt;"", YEAR(I15) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G15,
+         "junior_only",
+         IF(OR(H15="", $O$1 &lt;= H15),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10833,7 +10980,19 @@
         <v>1983</v>
       </c>
       <c r="N16" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F16,
+   "hidden",
+   IF(AND(I16&lt;&gt;"", YEAR(I16) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G16,
+         "junior_only",
+         IF(OR(H16="", $O$1 &lt;= H16),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10863,7 +11022,19 @@
         <v>1980</v>
       </c>
       <c r="N17" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F17,
+   "hidden",
+   IF(AND(I17&lt;&gt;"", YEAR(I17) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G17,
+         "junior_only",
+         IF(OR(H17="", $O$1 &lt;= H17),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10893,7 +11064,19 @@
         <v>1993</v>
       </c>
       <c r="N18" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F18,
+   "hidden",
+   IF(AND(I18&lt;&gt;"", YEAR(I18) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G18,
+         "junior_only",
+         IF(OR(H18="", $O$1 &lt;= H18),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10922,11 +11105,23 @@
       <c r="H19" s="5">
         <v>1982</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="10">
         <v>45781</v>
       </c>
       <c r="N19" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F19,
+   "hidden",
+   IF(AND(I19&lt;&gt;"", YEAR(I19) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G19,
+         "junior_only",
+         IF(OR(H19="", $O$1 &lt;= H19),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10956,7 +11151,19 @@
         <v>1983</v>
       </c>
       <c r="N20" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F20,
+   "hidden",
+   IF(AND(I20&lt;&gt;"", YEAR(I20) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G20,
+         "junior_only",
+         IF(OR(H20="", $O$1 &lt;= H20),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -10986,7 +11193,19 @@
         <v>1982</v>
       </c>
       <c r="N21" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F21,
+   "hidden",
+   IF(AND(I21&lt;&gt;"", YEAR(I21) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G21,
+         "junior_only",
+         IF(OR(H21="", $O$1 &lt;= H21),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -11015,11 +11234,23 @@
       <c r="H22" s="5">
         <v>1980</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="10">
         <v>39066</v>
       </c>
       <c r="N22" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F22,
+   "hidden",
+   IF(AND(I22&lt;&gt;"", YEAR(I22) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G22,
+         "junior_only",
+         IF(OR(H22="", $O$1 &lt;= H22),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -11049,7 +11280,19 @@
         <v>1981</v>
       </c>
       <c r="N23" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F23,
+   "hidden",
+   IF(AND(I23&lt;&gt;"", YEAR(I23) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G23,
+         "junior_only",
+         IF(OR(H23="", $O$1 &lt;= H23),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -11079,7 +11322,19 @@
         <v>1986</v>
       </c>
       <c r="N24" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F24,
+   "hidden",
+   IF(AND(I24&lt;&gt;"", YEAR(I24) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G24,
+         "junior_only",
+         IF(OR(H24="", $O$1 &lt;= H24),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -11108,11 +11363,23 @@
       <c r="H25" s="5">
         <v>1980</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I25" s="10">
         <v>29799</v>
       </c>
       <c r="N25" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F25,
+   "hidden",
+   IF(AND(I25&lt;&gt;"", YEAR(I25) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G25,
+         "junior_only",
+         IF(OR(H25="", $O$1 &lt;= H25),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -11142,7 +11409,19 @@
         <v>1980</v>
       </c>
       <c r="N26" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F26,
+   "hidden",
+   IF(AND(I26&lt;&gt;"", YEAR(I26) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G26,
+         "junior_only",
+         IF(OR(H26="", $O$1 &lt;= H26),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -11172,7 +11451,19 @@
         <v>1992</v>
       </c>
       <c r="N27" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F27,
+   "hidden",
+   IF(AND(I27&lt;&gt;"", YEAR(I27) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G27,
+         "junior_only",
+         IF(OR(H27="", $O$1 &lt;= H27),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -11202,7 +11493,19 @@
         <v>1991</v>
       </c>
       <c r="N28" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F28,
+   "hidden",
+   IF(AND(I28&lt;&gt;"", YEAR(I28) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G28,
+         "junior_only",
+         IF(OR(H28="", $O$1 &lt;= H28),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
@@ -11232,21 +11535,82 @@
         <v>1989</v>
       </c>
       <c r="N29" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($O$1 &lt; F29,
+   "hidden",
+   IF(AND(I29&lt;&gt;"", YEAR(I29) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G29,
+         "junior_only",
+         IF(OR(H29="", $O$1 &lt;= H29),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
         <v>eligible</v>
       </c>
     </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="E30" s="10">
+        <v>17951</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1971</v>
+      </c>
+      <c r="G30" s="5">
+        <v>1971</v>
+      </c>
+      <c r="H30" s="5">
+        <v>1985</v>
+      </c>
+      <c r="I30" s="10">
+        <v>43605</v>
+      </c>
+      <c r="N30" s="5" t="str">
+        <f>IF($O$1 &lt; F30,
+   "hidden",
+   IF(AND(I30&lt;&gt;"", YEAR(I30) &lt;= $O$1),
+      "deceased",
+      IF($O$1 &lt; G30,
+         "junior_only",
+         IF(OR(H30="", $O$1 &lt;= H30),
+            "eligible",
+            "retired"
+         )
+      )
+   )
+)</f>
+        <v>eligible</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O29">
+    <sortCondition ref="A10:A29"/>
+  </sortState>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:X29"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -13424,6 +13788,80 @@
         <v>64</v>
       </c>
     </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>1980</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="D30" s="5">
+        <v>83</v>
+      </c>
+      <c r="E30" s="5">
+        <v>83</v>
+      </c>
+      <c r="F30" s="5">
+        <v>72</v>
+      </c>
+      <c r="G30" s="5">
+        <v>68</v>
+      </c>
+      <c r="H30" s="5">
+        <v>60</v>
+      </c>
+      <c r="I30" s="5">
+        <v>86</v>
+      </c>
+      <c r="J30" s="5">
+        <v>72</v>
+      </c>
+      <c r="K30" s="5">
+        <v>90</v>
+      </c>
+      <c r="L30" s="5">
+        <v>82</v>
+      </c>
+      <c r="M30" s="5">
+        <v>95</v>
+      </c>
+      <c r="N30" s="5">
+        <v>98</v>
+      </c>
+      <c r="O30" s="5">
+        <v>85</v>
+      </c>
+      <c r="P30" s="5">
+        <v>75</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>94</v>
+      </c>
+      <c r="R30" s="5">
+        <v>65</v>
+      </c>
+      <c r="S30" s="5">
+        <v>30</v>
+      </c>
+      <c r="T30" s="5">
+        <v>92</v>
+      </c>
+      <c r="U30" s="5">
+        <v>88</v>
+      </c>
+      <c r="V30" s="5">
+        <v>82</v>
+      </c>
+      <c r="W30" s="5">
+        <v>97</v>
+      </c>
+      <c r="X30" s="5">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13458,46 +13896,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>486</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>539</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>501</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>502</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>504</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>505</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>506</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>507</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>618</v>
       </c>
     </row>
@@ -13965,7 +14403,7 @@
       <c r="D13" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>602</v>
       </c>
       <c r="G13" s="5">
@@ -14926,7 +15364,7 @@
       <c r="L36" s="5">
         <v>60</v>
       </c>
-      <c r="M36" s="14">
+      <c r="M36" s="13">
         <v>1</v>
       </c>
     </row>
@@ -14964,7 +15402,7 @@
       <c r="L37" s="5">
         <v>38</v>
       </c>
-      <c r="M37" s="15">
+      <c r="M37" s="14">
         <v>2</v>
       </c>
     </row>
@@ -15040,7 +15478,7 @@
       <c r="L39" s="5">
         <v>44</v>
       </c>
-      <c r="M39" s="16">
+      <c r="M39" s="15">
         <v>3</v>
       </c>
     </row>
@@ -15154,7 +15592,7 @@
       <c r="L42" s="5">
         <v>38</v>
       </c>
-      <c r="M42" s="14">
+      <c r="M42" s="13">
         <v>1</v>
       </c>
     </row>
@@ -15192,7 +15630,7 @@
       <c r="L43" s="5">
         <v>48</v>
       </c>
-      <c r="M43" s="15">
+      <c r="M43" s="14">
         <v>2</v>
       </c>
     </row>
@@ -15230,7 +15668,7 @@
       <c r="L44" s="5">
         <v>31</v>
       </c>
-      <c r="M44" s="16">
+      <c r="M44" s="15">
         <v>3</v>
       </c>
     </row>
@@ -15271,7 +15709,7 @@
       <c r="L45" s="5">
         <v>50</v>
       </c>
-      <c r="M45" s="14">
+      <c r="M45" s="13">
         <v>1</v>
       </c>
     </row>
@@ -15312,7 +15750,7 @@
       <c r="L46" s="5">
         <v>59</v>
       </c>
-      <c r="M46" s="14">
+      <c r="M46" s="13">
         <v>1</v>
       </c>
     </row>
@@ -15353,7 +15791,7 @@
       <c r="L47" s="5">
         <v>54</v>
       </c>
-      <c r="M47" s="15">
+      <c r="M47" s="14">
         <v>2</v>
       </c>
     </row>
@@ -15394,7 +15832,7 @@
       <c r="L48" s="5">
         <v>37</v>
       </c>
-      <c r="M48" s="16">
+      <c r="M48" s="15">
         <v>3</v>
       </c>
     </row>
@@ -16401,7 +16839,7 @@
       <c r="L73" s="5">
         <v>27</v>
       </c>
-      <c r="M73" s="16">
+      <c r="M73" s="15">
         <v>3</v>
       </c>
     </row>
@@ -16515,7 +16953,7 @@
       <c r="L76" s="5">
         <v>121</v>
       </c>
-      <c r="M76" s="15">
+      <c r="M76" s="14">
         <v>2</v>
       </c>
     </row>
@@ -16591,7 +17029,7 @@
       <c r="L78" s="5">
         <v>67</v>
       </c>
-      <c r="M78" s="14">
+      <c r="M78" s="13">
         <v>1</v>
       </c>
     </row>
@@ -16629,7 +17067,7 @@
       <c r="L79" s="5">
         <v>38</v>
       </c>
-      <c r="M79" s="16">
+      <c r="M79" s="15">
         <v>3</v>
       </c>
     </row>
@@ -16705,7 +17143,7 @@
       <c r="L81" s="5">
         <v>53</v>
       </c>
-      <c r="M81" s="14">
+      <c r="M81" s="13">
         <v>1</v>
       </c>
     </row>
@@ -17340,7 +17778,7 @@
       <c r="L97" s="5">
         <v>60</v>
       </c>
-      <c r="M97" s="14">
+      <c r="M97" s="13">
         <v>1</v>
       </c>
     </row>
@@ -17381,7 +17819,7 @@
       <c r="L98" s="5">
         <v>73</v>
       </c>
-      <c r="M98" s="15">
+      <c r="M98" s="14">
         <v>2</v>
       </c>
     </row>
@@ -17422,7 +17860,7 @@
       <c r="L99" s="5">
         <v>52</v>
       </c>
-      <c r="M99" s="15">
+      <c r="M99" s="14">
         <v>2</v>
       </c>
     </row>
@@ -17463,7 +17901,7 @@
       <c r="L100" s="5">
         <v>39</v>
       </c>
-      <c r="M100" s="15">
+      <c r="M100" s="14">
         <v>2</v>
       </c>
     </row>
@@ -17504,7 +17942,7 @@
       <c r="L101" s="5">
         <v>47</v>
       </c>
-      <c r="M101" s="15">
+      <c r="M101" s="14">
         <v>2</v>
       </c>
     </row>
@@ -17545,7 +17983,7 @@
       <c r="L102" s="5">
         <v>48</v>
       </c>
-      <c r="M102" s="16">
+      <c r="M102" s="15">
         <v>3</v>
       </c>
     </row>
@@ -17586,7 +18024,7 @@
       <c r="L103" s="5">
         <v>33</v>
       </c>
-      <c r="M103" s="16">
+      <c r="M103" s="15">
         <v>3</v>
       </c>
     </row>
@@ -17627,7 +18065,7 @@
       <c r="L104" s="5">
         <v>49</v>
       </c>
-      <c r="M104" s="16">
+      <c r="M104" s="15">
         <v>3</v>
       </c>
     </row>
@@ -19158,7 +19596,7 @@
       <c r="L142" s="5">
         <v>57</v>
       </c>
-      <c r="M142" s="14">
+      <c r="M142" s="13">
         <v>1</v>
       </c>
     </row>
@@ -19175,7 +19613,7 @@
       <c r="D143" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="F143" s="17" t="s">
+      <c r="F143" s="16" t="s">
         <v>75</v>
       </c>
       <c r="G143" s="5">
@@ -19213,7 +19651,7 @@
       <c r="D144" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="F144" s="17" t="s">
+      <c r="F144" s="16" t="s">
         <v>75</v>
       </c>
       <c r="G144" s="5">
@@ -20247,7 +20685,7 @@
       <c r="L169" s="5">
         <v>61</v>
       </c>
-      <c r="M169" s="14">
+      <c r="M169" s="13">
         <v>1</v>
       </c>
     </row>
@@ -20288,7 +20726,7 @@
       <c r="L170" s="5">
         <v>64</v>
       </c>
-      <c r="M170" s="14">
+      <c r="M170" s="13">
         <v>1</v>
       </c>
     </row>
@@ -20329,7 +20767,7 @@
       <c r="L171" s="5">
         <v>55</v>
       </c>
-      <c r="M171" s="15">
+      <c r="M171" s="14">
         <v>2</v>
       </c>
     </row>
@@ -20370,7 +20808,7 @@
       <c r="L172" s="5">
         <v>34</v>
       </c>
-      <c r="M172" s="16">
+      <c r="M172" s="15">
         <v>3</v>
       </c>
     </row>
@@ -20411,7 +20849,7 @@
       <c r="L173" s="5">
         <v>25</v>
       </c>
-      <c r="M173" s="16">
+      <c r="M173" s="15">
         <v>3</v>
       </c>
     </row>
@@ -20452,7 +20890,7 @@
       <c r="L174" s="5">
         <v>47</v>
       </c>
-      <c r="M174" s="16">
+      <c r="M174" s="15">
         <v>3</v>
       </c>
     </row>
@@ -21187,7 +21625,7 @@
       <c r="L192" s="5">
         <v>79</v>
       </c>
-      <c r="M192" s="14">
+      <c r="M192" s="13">
         <v>1</v>
       </c>
     </row>
@@ -21225,7 +21663,7 @@
       <c r="L193" s="5">
         <v>78</v>
       </c>
-      <c r="M193" s="14">
+      <c r="M193" s="13">
         <v>1</v>
       </c>
     </row>
@@ -21263,7 +21701,7 @@
       <c r="L194" s="5">
         <v>54</v>
       </c>
-      <c r="M194" s="14">
+      <c r="M194" s="13">
         <v>1</v>
       </c>
     </row>
@@ -21301,7 +21739,7 @@
       <c r="L195" s="5">
         <v>33</v>
       </c>
-      <c r="M195" s="16">
+      <c r="M195" s="15">
         <v>3</v>
       </c>
     </row>
@@ -21757,7 +22195,7 @@
       <c r="L207" s="5">
         <v>52</v>
       </c>
-      <c r="M207" s="15">
+      <c r="M207" s="14">
         <v>2</v>
       </c>
     </row>
@@ -21874,7 +22312,7 @@
       <c r="L210" s="5">
         <v>76</v>
       </c>
-      <c r="M210" s="14">
+      <c r="M210" s="13">
         <v>1</v>
       </c>
     </row>
@@ -21915,7 +22353,7 @@
       <c r="L211" s="5">
         <v>74</v>
       </c>
-      <c r="M211" s="14">
+      <c r="M211" s="13">
         <v>1</v>
       </c>
     </row>
@@ -21956,7 +22394,7 @@
       <c r="L212" s="5">
         <v>81</v>
       </c>
-      <c r="M212" s="14">
+      <c r="M212" s="13">
         <v>1</v>
       </c>
     </row>
@@ -21997,7 +22435,7 @@
       <c r="L213" s="5">
         <v>55</v>
       </c>
-      <c r="M213" s="14">
+      <c r="M213" s="13">
         <v>1</v>
       </c>
     </row>
@@ -22038,7 +22476,7 @@
       <c r="L214" s="5">
         <v>71.5</v>
       </c>
-      <c r="M214" s="15">
+      <c r="M214" s="14">
         <v>2</v>
       </c>
     </row>
@@ -22079,7 +22517,7 @@
       <c r="L215" s="5">
         <v>105</v>
       </c>
-      <c r="M215" s="15">
+      <c r="M215" s="14">
         <v>2</v>
       </c>
     </row>
@@ -22120,7 +22558,7 @@
       <c r="L216" s="5">
         <v>45</v>
       </c>
-      <c r="M216" s="15">
+      <c r="M216" s="14">
         <v>2</v>
       </c>
     </row>
@@ -22161,7 +22599,7 @@
       <c r="L217" s="5">
         <v>39</v>
       </c>
-      <c r="M217" s="16">
+      <c r="M217" s="15">
         <v>3</v>
       </c>
     </row>
@@ -23478,7 +23916,7 @@
       <c r="L250" s="5">
         <v>78</v>
       </c>
-      <c r="M250" s="14">
+      <c r="M250" s="13">
         <v>1</v>
       </c>
     </row>
@@ -23516,7 +23954,7 @@
       <c r="L251" s="5">
         <v>97</v>
       </c>
-      <c r="M251" s="14">
+      <c r="M251" s="13">
         <v>1</v>
       </c>
     </row>
@@ -23554,7 +23992,7 @@
       <c r="L252" s="5">
         <v>40</v>
       </c>
-      <c r="M252" s="15">
+      <c r="M252" s="14">
         <v>2</v>
       </c>
     </row>
@@ -23592,7 +24030,7 @@
       <c r="L253" s="5">
         <v>33</v>
       </c>
-      <c r="M253" s="16">
+      <c r="M253" s="15">
         <v>3</v>
       </c>
     </row>
@@ -23782,7 +24220,7 @@
       <c r="L258" s="5">
         <v>101</v>
       </c>
-      <c r="M258" s="14">
+      <c r="M258" s="13">
         <v>1</v>
       </c>
     </row>
@@ -23823,7 +24261,7 @@
       <c r="L259" s="5">
         <v>52</v>
       </c>
-      <c r="M259" s="14">
+      <c r="M259" s="13">
         <v>1</v>
       </c>
     </row>
@@ -23864,7 +24302,7 @@
       <c r="L260" s="5">
         <v>57</v>
       </c>
-      <c r="M260" s="15">
+      <c r="M260" s="14">
         <v>2</v>
       </c>
     </row>
@@ -24956,7 +25394,7 @@
       <c r="L287" s="5">
         <v>42</v>
       </c>
-      <c r="M287" s="15">
+      <c r="M287" s="14">
         <v>2</v>
       </c>
     </row>
@@ -25201,7 +25639,7 @@
       <c r="D294" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="F294" s="17" t="s">
+      <c r="F294" s="16" t="s">
         <v>601</v>
       </c>
       <c r="G294" s="5">
@@ -25260,7 +25698,7 @@
       <c r="L295" s="5">
         <v>44</v>
       </c>
-      <c r="M295" s="14">
+      <c r="M295" s="13">
         <v>1</v>
       </c>
     </row>
@@ -25678,7 +26116,7 @@
       <c r="L306" s="5">
         <v>52</v>
       </c>
-      <c r="M306" s="14">
+      <c r="M306" s="13">
         <v>1</v>
       </c>
     </row>
@@ -25757,7 +26195,7 @@
       <c r="L308" s="5">
         <v>45</v>
       </c>
-      <c r="M308" s="16">
+      <c r="M308" s="15">
         <v>3</v>
       </c>
     </row>
@@ -25798,7 +26236,7 @@
       <c r="L309" s="5">
         <v>49</v>
       </c>
-      <c r="M309" s="16">
+      <c r="M309" s="15">
         <v>3</v>
       </c>
     </row>
@@ -25839,7 +26277,7 @@
       <c r="L310" s="5">
         <v>27</v>
       </c>
-      <c r="M310" s="16">
+      <c r="M310" s="15">
         <v>3</v>
       </c>
     </row>
@@ -25880,7 +26318,7 @@
       <c r="L311" s="5">
         <v>38</v>
       </c>
-      <c r="M311" s="16">
+      <c r="M311" s="15">
         <v>3</v>
       </c>
     </row>
@@ -26735,7 +27173,7 @@
       <c r="L332" s="5">
         <v>55</v>
       </c>
-      <c r="M332" s="15">
+      <c r="M332" s="14">
         <v>2</v>
       </c>
     </row>
@@ -26852,7 +27290,7 @@
       <c r="L335" s="5">
         <v>99</v>
       </c>
-      <c r="M335" s="14">
+      <c r="M335" s="13">
         <v>1</v>
       </c>
     </row>
@@ -26893,7 +27331,7 @@
       <c r="L336" s="5">
         <v>71</v>
       </c>
-      <c r="M336" s="14">
+      <c r="M336" s="13">
         <v>1</v>
       </c>
     </row>
@@ -26934,7 +27372,7 @@
       <c r="L337" s="5">
         <v>44</v>
       </c>
-      <c r="M337" s="14">
+      <c r="M337" s="13">
         <v>1</v>
       </c>
     </row>
@@ -26975,7 +27413,7 @@
       <c r="L338" s="5">
         <v>76</v>
       </c>
-      <c r="M338" s="14">
+      <c r="M338" s="13">
         <v>1</v>
       </c>
     </row>
@@ -27016,7 +27454,7 @@
       <c r="L339" s="5">
         <v>49</v>
       </c>
-      <c r="M339" s="15">
+      <c r="M339" s="14">
         <v>2</v>
       </c>
     </row>
@@ -27057,7 +27495,7 @@
       <c r="L340" s="5">
         <v>56</v>
       </c>
-      <c r="M340" s="15">
+      <c r="M340" s="14">
         <v>2</v>
       </c>
     </row>
@@ -27098,7 +27536,7 @@
       <c r="L341" s="5">
         <v>43</v>
       </c>
-      <c r="M341" s="16">
+      <c r="M341" s="15">
         <v>3</v>
       </c>
     </row>
@@ -27139,7 +27577,7 @@
       <c r="L342" s="5">
         <v>46</v>
       </c>
-      <c r="M342" s="16">
+      <c r="M342" s="15">
         <v>3</v>
       </c>
     </row>
@@ -27180,7 +27618,7 @@
       <c r="L343" s="5">
         <v>49</v>
       </c>
-      <c r="M343" s="16">
+      <c r="M343" s="15">
         <v>3</v>
       </c>
     </row>
@@ -27221,7 +27659,7 @@
       <c r="L344" s="5">
         <v>40</v>
       </c>
-      <c r="M344" s="16">
+      <c r="M344" s="15">
         <v>3</v>
       </c>
     </row>
@@ -27262,7 +27700,7 @@
       <c r="L345" s="5">
         <v>69</v>
       </c>
-      <c r="M345" s="16">
+      <c r="M345" s="15">
         <v>3</v>
       </c>
     </row>
@@ -27303,7 +27741,7 @@
       <c r="L346" s="5">
         <v>40</v>
       </c>
-      <c r="M346" s="16">
+      <c r="M346" s="15">
         <v>3</v>
       </c>
     </row>
@@ -27344,7 +27782,7 @@
       <c r="L347" s="5">
         <v>53</v>
       </c>
-      <c r="M347" s="16">
+      <c r="M347" s="15">
         <v>3</v>
       </c>
     </row>

</xml_diff>